<commit_message>
Fixes #81 - Implemented the latest Excel import template.
</commit_message>
<xml_diff>
--- a/spec/fixtures/imports/excel_xl_import_test.xlsx
+++ b/spec/fixtures/imports/excel_xl_import_test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>title</t>
   </si>
@@ -69,9 +69,6 @@
     <t>image-source</t>
   </si>
   <si>
-    <t>http://id.loc.gov/vocabulary/resourceTypes/img | http://id.loc.gov/vocabulary/resourceTypes/mix</t>
-  </si>
-  <si>
     <t>Decenber 10, 2016 @{begin=2016-12-10 ; end=2016-12-10 }</t>
   </si>
   <si>
@@ -94,6 +91,51 @@
   </si>
   <si>
     <t>file_2.jpg</t>
+  </si>
+  <si>
+    <t>mixed material | still image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eng  - English|zxx  - No linguistic content; Not applicable </t>
+  </si>
+  <si>
+    <t>SUBJECT:TOPIC</t>
+  </si>
+  <si>
+    <t>AGENT:CREATOR</t>
+  </si>
+  <si>
+    <t>IDENTIFIER:DOI</t>
+  </si>
+  <si>
+    <t>NOTE:NOTE</t>
+  </si>
+  <si>
+    <t>copyright status</t>
+  </si>
+  <si>
+    <t>US - United States of America</t>
+  </si>
+  <si>
+    <t>copyrighted</t>
+  </si>
+  <si>
+    <t>subject:spatial</t>
+  </si>
+  <si>
+    <t>SUBJECT:SPATIAL</t>
+  </si>
+  <si>
+    <t>file path</t>
+  </si>
+  <si>
+    <t>copyright jurisdiction</t>
+  </si>
+  <si>
+    <t>agent:contributor</t>
+  </si>
+  <si>
+    <t>AGENT:CONTRIBUTOR</t>
   </si>
 </sst>
 </file>
@@ -151,17 +193,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="13"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13.2"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -182,8 +224,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -214,14 +272,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -234,6 +292,14 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -246,6 +312,14 @@
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -575,18 +649,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="3" max="4" width="15.5" customWidth="1"/>
+    <col min="14" max="14" width="39.6640625" customWidth="1"/>
+    <col min="15" max="15" width="30" customWidth="1"/>
+    <col min="17" max="17" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16">
+    <row r="1" spans="1:19" ht="16">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -597,89 +674,131 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="R1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" ht="16">
+    <row r="2" spans="1:19" ht="16">
       <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="6" t="s">
         <v>18</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="K2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="4" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="I2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="N2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
         <v>21</v>
       </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixes #67 - Updated related resource implementation for Batch Import.
</commit_message>
<xml_diff>
--- a/spec/fixtures/imports/excel_xl_import_test.xlsx
+++ b/spec/fixtures/imports/excel_xl_import_test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>title</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t>AGENT:CONTRIBUTOR</t>
+  </si>
+  <si>
+    <t>related resource</t>
+  </si>
+  <si>
+    <t>RELATED RESOURCE @{relatedType=relation; url=http://test.com/related_resource/relation}</t>
   </si>
 </sst>
 </file>
@@ -224,8 +230,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -279,7 +287,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="41">
+  <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -300,6 +308,7 @@
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -320,6 +329,7 @@
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -649,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -663,7 +673,7 @@
     <col min="17" max="17" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="16">
+    <row r="1" spans="1:20" ht="16">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -721,8 +731,11 @@
       <c r="S1" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="T1" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" ht="16">
+    <row r="2" spans="1:20" ht="16">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -767,8 +780,11 @@
       <c r="S2" s="7" t="s">
         <v>32</v>
       </c>
+      <c r="T2" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:20">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -785,7 +801,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:20">
       <c r="A4" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Fixes #67 - Implemented blank node with edit form support for related resource. (#76)
* Fixes #67 - Implemented blank node support with edit form for related
resource.

* Fixes #67 - Updated related resource implementation for Batch Import.
</commit_message>
<xml_diff>
--- a/spec/fixtures/imports/excel_xl_import_test.xlsx
+++ b/spec/fixtures/imports/excel_xl_import_test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>title</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t>AGENT:CONTRIBUTOR</t>
+  </si>
+  <si>
+    <t>related resource</t>
+  </si>
+  <si>
+    <t>RELATED RESOURCE @{relatedType=relation; url=http://test.com/related_resource/relation}</t>
   </si>
 </sst>
 </file>
@@ -224,8 +230,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -279,7 +287,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="41">
+  <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -300,6 +308,7 @@
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -320,6 +329,7 @@
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -649,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -663,7 +673,7 @@
     <col min="17" max="17" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="16">
+    <row r="1" spans="1:20" ht="16">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -721,8 +731,11 @@
       <c r="S1" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="T1" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" ht="16">
+    <row r="2" spans="1:20" ht="16">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -767,8 +780,11 @@
       <c r="S2" s="7" t="s">
         <v>32</v>
       </c>
+      <c r="T2" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:20">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -785,7 +801,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:20">
       <c r="A4" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Fixes #84 - Implemented the new rights metadata model with local customized visibilities.
</commit_message>
<xml_diff>
--- a/spec/fixtures/imports/excel_xl_import_test.xlsx
+++ b/spec/fixtures/imports/excel_xl_import_test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>title</t>
   </si>
@@ -142,6 +142,18 @@
   </si>
   <si>
     <t>RELATED RESOURCE @{relatedType=relation; url=http://test.com/related_resource/relation}</t>
+  </si>
+  <si>
+    <t>rights holder</t>
+  </si>
+  <si>
+    <t>AGENT:RIGHTS_HOLDER</t>
+  </si>
+  <si>
+    <t>license</t>
+  </si>
+  <si>
+    <t>MIT</t>
   </si>
 </sst>
 </file>
@@ -230,7 +242,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -274,8 +286,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -286,8 +304,11 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -309,6 +330,9 @@
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -330,6 +354,9 @@
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -659,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -671,9 +698,12 @@
     <col min="14" max="14" width="39.6640625" customWidth="1"/>
     <col min="15" max="15" width="30" customWidth="1"/>
     <col min="17" max="17" width="26.83203125" customWidth="1"/>
+    <col min="18" max="18" width="14.83203125" customWidth="1"/>
+    <col min="19" max="21" width="16.83203125" customWidth="1"/>
+    <col min="22" max="22" width="77" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="16">
+    <row r="1" spans="1:22" ht="16">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -732,10 +762,16 @@
         <v>30</v>
       </c>
       <c r="T1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="16">
+    <row r="2" spans="1:22" ht="30">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -780,11 +816,17 @@
       <c r="S2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="V2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -801,7 +843,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:22">
       <c r="A4" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Fixed #84, #85, #92, #59 - Implemented the new rights metadata model with local customized visibilities. (#108)
* Fixes #84 - Implemented the new rights metadata model with local
customized visibilities.

* Fixes #59 - Ported Suppress Discovery feature.

* Fises #92 - Ported Metadata-Only feature, added icon display for
Culturally-Sensitive visibility.

* Fixes #84 - Updated to use the latest hyrax pattern in solr_doc to fetch
field values.

* Fixes #84 - Corrected rubocop style check violations.
</commit_message>
<xml_diff>
--- a/spec/fixtures/imports/excel_xl_import_test.xlsx
+++ b/spec/fixtures/imports/excel_xl_import_test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>title</t>
   </si>
@@ -142,6 +142,18 @@
   </si>
   <si>
     <t>RELATED RESOURCE @{relatedType=relation; url=http://test.com/related_resource/relation}</t>
+  </si>
+  <si>
+    <t>rights holder</t>
+  </si>
+  <si>
+    <t>AGENT:RIGHTS_HOLDER</t>
+  </si>
+  <si>
+    <t>license</t>
+  </si>
+  <si>
+    <t>MIT</t>
   </si>
 </sst>
 </file>
@@ -230,7 +242,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -274,8 +286,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -286,8 +304,11 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -309,6 +330,9 @@
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -330,6 +354,9 @@
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -659,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -671,9 +698,12 @@
     <col min="14" max="14" width="39.6640625" customWidth="1"/>
     <col min="15" max="15" width="30" customWidth="1"/>
     <col min="17" max="17" width="26.83203125" customWidth="1"/>
+    <col min="18" max="18" width="14.83203125" customWidth="1"/>
+    <col min="19" max="21" width="16.83203125" customWidth="1"/>
+    <col min="22" max="22" width="77" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="16">
+    <row r="1" spans="1:22" ht="16">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -732,10 +762,16 @@
         <v>30</v>
       </c>
       <c r="T1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="16">
+    <row r="2" spans="1:22" ht="30">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -780,11 +816,17 @@
       <c r="S2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="V2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -801,7 +843,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:22">
       <c r="A4" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Fixes #111 - Implemented the file use model.
</commit_message>
<xml_diff>
--- a/spec/fixtures/imports/excel_xl_import_test.xlsx
+++ b/spec/fixtures/imports/excel_xl_import_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="16280" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="excel_xl_import_test.xlsx" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
   <si>
     <t>title</t>
   </si>
@@ -66,9 +66,6 @@
     <t>type of resource</t>
   </si>
   <si>
-    <t>image-source</t>
-  </si>
-  <si>
     <t>Decenber 10, 2016 @{begin=2016-12-10 ; end=2016-12-10 }</t>
   </si>
   <si>
@@ -154,6 +151,15 @@
   </si>
   <si>
     <t>MIT</t>
+  </si>
+  <si>
+    <t>OriginalFile</t>
+  </si>
+  <si>
+    <t>image.jpg</t>
+  </si>
+  <si>
+    <t>PreservationMasterFile</t>
   </si>
 </sst>
 </file>
@@ -242,8 +248,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -308,7 +316,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="51">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -333,6 +341,7 @@
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -357,6 +366,7 @@
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -688,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -714,7 +724,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
@@ -735,10 +745,10 @@
         <v>6</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>11</v>
@@ -756,27 +766,27 @@
         <v>14</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="30">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -784,80 +794,86 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
         <v>26</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" t="s">
-        <v>28</v>
-      </c>
       <c r="P2" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="S2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="S2" s="7" t="s">
-        <v>32</v>
-      </c>
       <c r="T2" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="U2" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="V2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:22">
       <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:22">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>22</v>
       </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
+      <c r="F4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>